<commit_message>
Updated eval tasks doc
</commit_message>
<xml_diff>
--- a/docs/H20 Task.xlsx
+++ b/docs/H20 Task.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5625" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -260,8 +255,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -388,8 +383,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,6 +470,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -741,6 +748,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +780,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{1E3440BA-097D-4E78-9633-F34AFA608A6C}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1075,29 +1085,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.19921875" customWidth="1"/>
-    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.25" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="40.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>43122</v>
       </c>
@@ -1116,14 +1126,14 @@
         <v>43218</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:5" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:5" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1167,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
@@ -1208,7 +1218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
@@ -1225,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -1242,7 +1252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>15</v>
       </c>
@@ -1276,7 +1286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>17</v>
       </c>
@@ -1293,7 +1303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>18</v>
       </c>
@@ -1310,13 +1320,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>34</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>35</v>
       </c>
@@ -1370,7 +1380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>36</v>
       </c>
@@ -1384,7 +1394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>37</v>
       </c>
@@ -1398,35 +1408,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25"/>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="25"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="25"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="25"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="25"/>
     </row>
-    <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>2</v>
       </c>
@@ -1443,7 +1453,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>27</v>
       </c>
@@ -1477,7 +1487,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>26</v>
       </c>
@@ -1494,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>25</v>
       </c>
@@ -1511,7 +1521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>24</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>22</v>
       </c>
@@ -1556,13 +1566,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
         <v>2</v>
       </c>
@@ -1579,7 +1589,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>34</v>
       </c>
@@ -1593,7 +1603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>35</v>
       </c>
@@ -1607,7 +1617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>36</v>
       </c>
@@ -1621,7 +1631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>37</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
         <v>16</v>
       </c>
@@ -1643,7 +1653,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
         <v>16</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
         <v>16</v>
       </c>
@@ -1659,7 +1669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
         <v>16</v>
       </c>
@@ -1674,30 +1684,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9B9568-22E5-4E70-BE77-F6302AEFBA99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>41</v>
       </c>
@@ -1721,7 +1731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>42</v>
       </c>
@@ -1729,7 +1739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>67</v>
       </c>
@@ -1737,7 +1747,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>68</v>
       </c>
@@ -1745,7 +1755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>69</v>
       </c>
@@ -1753,13 +1763,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1777,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>48</v>
       </c>
@@ -1775,7 +1785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>49</v>
       </c>
@@ -1783,7 +1793,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>50</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>67</v>
       </c>
@@ -1799,7 +1809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>70</v>
       </c>
@@ -1807,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>71</v>
       </c>
@@ -1815,7 +1825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>72</v>
       </c>
@@ -1823,7 +1833,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>73</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>74</v>
       </c>
@@ -1839,7 +1849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>75</v>
       </c>
@@ -1847,13 +1857,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>2</v>
       </c>
@@ -1861,7 +1871,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>53</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>54</v>
       </c>
@@ -1877,7 +1887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>55</v>
       </c>
@@ -1885,7 +1895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>56</v>
       </c>
@@ -1893,7 +1903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>57</v>
       </c>
@@ -1901,7 +1911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>58</v>
       </c>
@@ -1909,7 +1919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>59</v>
       </c>
@@ -1917,13 +1927,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
         <v>2</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>76</v>
       </c>
@@ -1939,7 +1949,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>77</v>
       </c>
@@ -1953,30 +1963,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33338822-9A74-40C0-AC16-84D05209DE05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>2</v>
       </c>
@@ -1984,69 +1994,69 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B10" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>2</v>
       </c>
@@ -2054,53 +2064,53 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B18" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>2</v>
       </c>
@@ -2108,69 +2118,69 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="B28" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>2</v>
       </c>
@@ -2178,47 +2188,48 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>16</v>
+      <c r="B36" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>